<commit_message>
Update before DFM changes
</commit_message>
<xml_diff>
--- a/Out of stock.xlsx
+++ b/Out of stock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dacut/Documents/Projects/Scoreboard/HDMI Breakout/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E1F380-7A54-DB4F-BA05-057040F19593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED2BA73-6D9E-5C41-AF5C-F52DD9881242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41080" yWindow="2980" windowWidth="27240" windowHeight="16440" xr2:uid="{B48A1C52-1C91-F547-9DFD-A1AB17EECB4C}"/>
+    <workbookView xWindow="7260" yWindow="2040" windowWidth="27240" windowHeight="16440" xr2:uid="{B48A1C52-1C91-F547-9DFD-A1AB17EECB4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
   <si>
     <t>CC0402MRX6S5BB106</t>
   </si>
@@ -165,6 +165,48 @@
   </si>
   <si>
     <t>C4345381</t>
+  </si>
+  <si>
+    <t>Quote Ok?</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>C5189822</t>
+  </si>
+  <si>
+    <t>Samwha Capacitor</t>
+  </si>
+  <si>
+    <t>CS2012X7R106M100NRE</t>
+  </si>
+  <si>
+    <t>C43473</t>
+  </si>
+  <si>
+    <t>Uni-Royal</t>
+  </si>
+  <si>
+    <t>0402WGF2212TCE</t>
+  </si>
+  <si>
+    <t>ERJPA2J331X</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>C427206</t>
+  </si>
+  <si>
+    <t>0402WGF4751TCE</t>
+  </si>
+  <si>
+    <t>C25901</t>
   </si>
 </sst>
 </file>
@@ -180,25 +222,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF212121"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
+      <sz val="12"/>
+      <color rgb="FF212121"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -565,207 +608,350 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1457BE41-792F-1743-9181-4038B07A8BC2}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.1640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="34" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="34" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="I2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="I3" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="I4" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="I5" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="I6" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="1" t="s">
         <v>41</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>